<commit_message>
Aggiornati sets.json e cards.json
</commit_message>
<xml_diff>
--- a/sets_template.xlsx
+++ b/sets_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dese9\Desktop\pokemon_app\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dese9\Documents\GitHub\Collezione-Pokemon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C98609C-64D5-45B6-9E03-2E61FCD75BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13356D3-A7BE-4B67-A44A-098B2D507CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{BCD853FE-3698-4A91-AD03-10CE1AA2820A}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>logo_diamante_e_perla_fronte_di_tempesta.webp</t>
   </si>
   <si>
-    <t>logo_diamante_e_perla_il_risveglio_dei_miti.webp</t>
-  </si>
-  <si>
     <t>logo_ex_power_keepers.webp</t>
   </si>
   <si>
@@ -840,13 +837,16 @@
   </si>
   <si>
     <t>logo_promo_stella_nera_swsh.png</t>
+  </si>
+  <si>
+    <t>logo_diamante_e_perla_il_risveglio_dei_miti.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -864,6 +864,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -904,11 +912,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1245,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC6E637-362A-4EF8-A056-5792EA1659FF}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,19 +1291,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2">
         <v>102</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1302,19 +1311,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2">
         <v>64</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1322,19 +1331,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2">
         <v>62</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1342,19 +1351,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2">
         <v>83</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1362,19 +1371,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2">
         <v>132</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1382,19 +1391,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2">
         <v>132</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1402,19 +1411,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2">
         <v>111</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1422,19 +1431,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2">
         <v>75</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1442,19 +1451,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2">
         <v>66</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1462,19 +1471,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2">
         <v>113</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1482,19 +1491,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2">
         <v>165</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1502,19 +1511,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2">
         <v>186</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1522,19 +1531,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2">
         <v>182</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1542,19 +1551,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2">
         <v>53</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1562,19 +1571,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2">
         <v>109</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1582,19 +1591,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2">
         <v>100</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1602,19 +1611,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2">
         <v>100</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1622,19 +1631,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="2">
         <v>97</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1642,19 +1651,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2">
         <v>102</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1662,19 +1671,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="2">
         <v>116</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1688,13 +1697,13 @@
         <v>111</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1708,13 +1717,13 @@
         <v>108</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1728,13 +1737,13 @@
         <v>107</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1742,19 +1751,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2">
         <v>145</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1762,19 +1771,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2">
         <v>114</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1788,13 +1797,13 @@
         <v>93</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,13 +1817,13 @@
         <v>111</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1822,19 +1831,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="2">
         <v>100</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1842,19 +1851,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="2">
         <v>101</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1862,19 +1871,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" s="2">
         <v>108</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1882,19 +1891,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="2">
         <v>40</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1902,19 +1911,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="2">
         <v>130</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1928,13 +1937,13 @@
         <v>124</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1948,13 +1957,13 @@
         <v>132</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1968,13 +1977,13 @@
         <v>106</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1988,13 +1997,13 @@
         <v>100</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2008,13 +2017,13 @@
         <v>146</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>26</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2022,18 +2031,18 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C39" s="2">
         <v>106</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2042,19 +2051,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C40" s="2">
         <v>56</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2071,10 +2080,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2082,7 +2091,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C42" s="2">
         <v>120</v>
@@ -2091,7 +2100,7 @@
         <v>15</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>24</v>
@@ -2102,7 +2111,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43" s="2">
         <v>153</v>
@@ -2111,7 +2120,7 @@
         <v>15</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>23</v>
@@ -2122,7 +2131,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C44" s="2">
         <v>111</v>
@@ -2131,7 +2140,7 @@
         <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>22</v>
@@ -2151,7 +2160,7 @@
         <v>18</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>21</v>
@@ -2162,7 +2171,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C46" s="2">
         <v>96</v>
@@ -2171,10 +2180,10 @@
         <v>18</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2182,7 +2191,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C47" s="2">
         <v>91</v>
@@ -2191,10 +2200,10 @@
         <v>18</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2202,7 +2211,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C48" s="2">
         <v>103</v>
@@ -2211,10 +2220,10 @@
         <v>18</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2222,7 +2231,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C49" s="2">
         <v>33</v>
@@ -2231,10 +2240,10 @@
         <v>18</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2251,7 +2260,7 @@
         <v>17</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>19</v>
@@ -2262,7 +2271,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C51" s="2">
         <v>98</v>
@@ -2271,10 +2280,10 @@
         <v>17</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2282,7 +2291,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C52" s="2">
         <v>102</v>
@@ -2291,10 +2300,10 @@
         <v>17</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2302,7 +2311,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" s="2">
         <v>103</v>
@@ -2311,10 +2320,10 @@
         <v>17</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2322,7 +2331,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" s="2">
         <v>111</v>
@@ -2331,10 +2340,10 @@
         <v>17</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2342,7 +2351,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C55" s="2">
         <v>128</v>
@@ -2351,10 +2360,10 @@
         <v>17</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2362,7 +2371,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C56" s="2">
         <v>21</v>
@@ -2371,10 +2380,10 @@
         <v>17</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2382,7 +2391,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C57" s="2">
         <v>153</v>
@@ -2391,10 +2400,10 @@
         <v>17</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2402,7 +2411,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C58" s="2">
         <v>138</v>
@@ -2411,10 +2420,10 @@
         <v>17</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2422,7 +2431,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C59" s="2">
         <v>122</v>
@@ -2431,10 +2440,10 @@
         <v>17</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2442,7 +2451,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C60" s="2">
         <v>105</v>
@@ -2451,10 +2460,10 @@
         <v>17</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2462,7 +2471,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C61" s="2">
         <v>140</v>
@@ -2471,10 +2480,10 @@
         <v>17</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2482,7 +2491,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C62" s="2">
         <v>116</v>
@@ -2491,10 +2500,10 @@
         <v>17</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2502,19 +2511,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C63" s="2">
         <v>39</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2522,16 +2531,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C64" s="2">
         <v>146</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>20</v>
@@ -2542,19 +2551,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C65" s="2">
         <v>109</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2562,19 +2571,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C66" s="2">
         <v>113</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2582,19 +2591,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C67" s="2">
         <v>122</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2602,19 +2611,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C68" s="2">
         <v>164</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2622,19 +2631,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C69" s="2">
         <v>110</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2642,19 +2651,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C70" s="2">
         <v>100</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2662,19 +2671,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C71" s="2">
         <v>164</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2682,19 +2691,19 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C72" s="2">
         <v>123</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2702,19 +2711,19 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C73" s="2">
         <v>115</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2722,19 +2731,19 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C74" s="2">
         <v>125</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2742,19 +2751,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C75" s="2">
         <v>116</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2762,19 +2771,19 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C76" s="2">
         <v>113</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2782,19 +2791,19 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C77" s="2">
         <v>213</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2802,19 +2811,19 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C78" s="2">
         <v>163</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2822,19 +2831,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C79" s="2">
         <v>169</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2842,19 +2851,19 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C80" s="2">
         <v>169</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2862,19 +2871,19 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C81" s="2">
         <v>78</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2882,19 +2891,19 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C82" s="2">
         <v>124</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2902,19 +2911,19 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C83" s="2">
         <v>173</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2922,19 +2931,19 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C84" s="2">
         <v>146</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2942,19 +2951,19 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C85" s="2">
         <v>183</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2962,19 +2971,19 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C86" s="2">
         <v>78</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2982,19 +2991,19 @@
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C87" s="2">
         <v>236</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3002,19 +3011,19 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C88" s="2">
         <v>196</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -3022,19 +3031,19 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C89" s="2">
         <v>18</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3042,19 +3051,19 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C90" s="2">
         <v>234</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3062,19 +3071,19 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C91" s="2">
         <v>258</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3082,19 +3091,19 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C92" s="2">
         <v>163</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3102,19 +3111,19 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C93" s="2">
         <v>271</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3122,19 +3131,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C94" s="2">
         <v>249</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3142,19 +3151,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C95" s="2">
         <v>216</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3162,19 +3171,19 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C96" s="2">
         <v>209</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3182,19 +3191,19 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C97" s="2">
         <v>201</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3202,19 +3211,19 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C98" s="2">
         <v>80</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3222,19 +3231,19 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C99" s="2">
         <v>203</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3242,19 +3251,19 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C100" s="2">
         <v>195</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3262,19 +3271,19 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C101" s="2">
         <v>183</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3282,19 +3291,19 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C102" s="2">
         <v>233</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3302,19 +3311,19 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C103" s="2">
         <v>237</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3322,19 +3331,19 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C104" s="2">
         <v>284</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3342,19 +3351,19 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C105" s="2">
         <v>216</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3362,19 +3371,19 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C106" s="2">
         <v>246</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3382,19 +3391,19 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C107" s="2">
         <v>88</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3402,19 +3411,19 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C108" s="2">
         <v>247</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -3422,19 +3431,19 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C109" s="2">
         <v>245</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3442,19 +3451,19 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C110" s="2">
         <v>230</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3462,19 +3471,19 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C111" s="2">
         <v>305</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -3482,19 +3491,19 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C112" s="2">
         <v>258</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3502,19 +3511,19 @@
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C113" s="2">
         <v>279</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3522,19 +3531,19 @@
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C114" s="2">
         <v>230</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3542,19 +3551,19 @@
         <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C115" s="2">
         <v>210</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3562,19 +3571,19 @@
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C116" s="2">
         <v>266</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3582,19 +3591,19 @@
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C117" s="2">
         <v>245</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3602,19 +3611,19 @@
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C118" s="2">
         <v>218</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3622,19 +3631,19 @@
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C119" s="2">
         <v>226</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3642,19 +3651,19 @@
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C120" s="2">
         <v>99</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3662,19 +3671,19 @@
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C121" s="2">
         <v>175</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3682,19 +3691,19 @@
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C122" s="2">
         <v>252</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3702,19 +3711,19 @@
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C123" s="2">
         <v>180</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3722,19 +3731,19 @@
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C124" s="2">
         <v>190</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3742,19 +3751,19 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C125" s="2">
         <v>244</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3762,19 +3771,19 @@
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C126" s="2">
         <v>172</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3782,19 +3791,19 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C127" s="2">
         <v>173</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3802,19 +3811,19 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C128" s="2">
         <v>226</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3822,19 +3831,19 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C129" s="2">
         <v>188</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>